<commit_message>
user can fetch and share calendars
</commit_message>
<xml_diff>
--- a/server-app/src/main/resources/Uploads/Book1.xlsx
+++ b/server-app/src/main/resources/Uploads/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahar\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F20C3913-74F4-483F-AD3B-18E9973CAD4E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A169E6E-4F21-4248-A20C-306FF4C001D9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{4809F01D-A732-413A-A150-A59C5FFBA6B0}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>First name</t>
   </si>
@@ -86,6 +85,15 @@
   </si>
   <si>
     <t>asdffgg</t>
+  </si>
+  <si>
+    <t>Pudasainy</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>Rohan9841@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -475,7 +483,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,11 +572,23 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="F6" s="3"/>
+      <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6">
+        <v>30082878</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F6" r:id="rId1" xr:uid="{E029E81F-8D1E-4C2B-8F5F-952559F0877B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
course group and custom group added
</commit_message>
<xml_diff>
--- a/server-app/src/main/resources/Uploads/Book1.xlsx
+++ b/server-app/src/main/resources/Uploads/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahar\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A169E6E-4F21-4248-A20C-306FF4C001D9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4572AC2-631E-4248-865D-3CEB810B7A1B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{4809F01D-A732-413A-A150-A59C5FFBA6B0}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>First name</t>
   </si>
@@ -54,24 +54,12 @@
     <t>Last downloaded from this course</t>
   </si>
   <si>
-    <t>Maharjan</t>
-  </si>
-  <si>
     <t>maharjr@warhawks.ulm.edu</t>
   </si>
   <si>
     <t>Rohan@sunquestproperties.com</t>
   </si>
   <si>
-    <t>asdaf</t>
-  </si>
-  <si>
-    <t>asdf</t>
-  </si>
-  <si>
-    <t>Rohan</t>
-  </si>
-  <si>
     <t>30079753</t>
   </si>
   <si>
@@ -84,9 +72,6 @@
     <t>1567713827</t>
   </si>
   <si>
-    <t>asdffgg</t>
-  </si>
-  <si>
     <t>Pudasainy</t>
   </si>
   <si>
@@ -94,6 +79,18 @@
   </si>
   <si>
     <t>Rohan9841@gmail.com</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Henry</t>
+  </si>
+  <si>
+    <t>Shirish</t>
+  </si>
+  <si>
+    <t>Dangol</t>
   </si>
 </sst>
 </file>
@@ -483,7 +480,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,55 +531,55 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
+        <v>19</v>
+      </c>
+      <c r="C5">
+        <v>1234567</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C6">
         <v>30082878</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>